<commit_message>
DCM and PGM commit on 20230925
</commit_message>
<xml_diff>
--- a/03.設計/画面設計書_STB.xlsx
+++ b/03.設計/画面設計書_STB.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micch\OneDrive\デスクトップ\PGP_source\03.設計\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micch\OneDrive\デスクトップ\PGP\03.設計\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13212" tabRatio="888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200" tabRatio="888"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="159" r:id="rId1"/>
@@ -256,14 +256,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>TM</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>画面設計書</t>
     <rPh sb="0" eb="5">
       <t>ガメンセッケイショ</t>
@@ -291,6 +283,14 @@
     <rPh sb="7" eb="10">
       <t>ヒョウジジ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MT</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -737,6 +737,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -758,6 +761,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,23 +794,50 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -798,54 +846,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4268,34 +4268,34 @@
     </row>
     <row r="6" spans="3:16" ht="49.2" customHeight="1">
       <c r="C6" s="7"/>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
       <c r="N6" s="8"/>
     </row>
     <row r="7" spans="3:16" ht="49.2" customHeight="1">
       <c r="C7" s="7"/>
-      <c r="D7" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
+      <c r="D7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
       <c r="N7" s="8"/>
     </row>
     <row r="8" spans="3:16" ht="22.5" customHeight="1" thickBot="1">
@@ -4314,80 +4314,80 @@
     </row>
     <row r="9" spans="3:16" ht="22.5" customHeight="1" thickTop="1"/>
     <row r="11" spans="3:16" ht="22.5" customHeight="1">
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27" t="s">
+      <c r="G11" s="27"/>
+      <c r="H11" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="3:16" ht="22.5" customHeight="1">
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="25" t="s">
+      <c r="G12" s="27"/>
+      <c r="H12" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="26"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="27"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="3:16" ht="22.5" customHeight="1">
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27" t="s">
+      <c r="G13" s="27"/>
+      <c r="H13" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
     </row>
     <row r="14" spans="3:16" ht="22.5" customHeight="1">
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="27" t="s">
+      <c r="G14" s="27"/>
+      <c r="H14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
     </row>
     <row r="15" spans="3:16" ht="22.5" customHeight="1">
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
     </row>
     <row r="16" spans="3:16" ht="22.5" customHeight="1">
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="30"/>
       <c r="N16" s="1" t="s">
         <v>27</v>
       </c>
@@ -4462,58 +4462,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
       <c r="P1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="33" t="str">
+      <c r="Q1" s="40" t="str">
         <f>D5</f>
-        <v>TM</v>
-      </c>
-      <c r="R1" s="33"/>
+        <v>MT</v>
+      </c>
+      <c r="R1" s="40"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
       <c r="P2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="34">
+      <c r="Q2" s="41">
         <f>B5</f>
         <v>45170</v>
       </c>
-      <c r="R2" s="33"/>
+      <c r="R2" s="40"/>
     </row>
     <row r="3" spans="1:18" ht="22.5" customHeight="1">
       <c r="A3" s="19"/>
@@ -4539,435 +4539,435 @@
       <c r="A4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
     </row>
     <row r="5" spans="1:18" ht="22.5" customHeight="1">
       <c r="A5" s="21">
         <v>1</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="35">
         <v>45170</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38" t="s">
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
     </row>
     <row r="6" spans="1:18" ht="22.5" customHeight="1">
       <c r="A6" s="22">
         <v>2</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
     </row>
     <row r="7" spans="1:18" ht="27" customHeight="1">
       <c r="A7" s="22">
         <v>3</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1">
       <c r="A8" s="22">
         <v>4</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1">
       <c r="A9" s="22">
         <v>5</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
     </row>
     <row r="10" spans="1:18" ht="27" customHeight="1">
       <c r="A10" s="22">
         <v>6</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1">
       <c r="A11" s="22">
         <v>7</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1">
       <c r="A12" s="22">
         <v>8</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
     </row>
     <row r="13" spans="1:18" ht="27" customHeight="1">
       <c r="A13" s="22">
         <v>9</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1">
       <c r="A14" s="22">
         <v>10</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1">
       <c r="A15" s="22">
         <v>11</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
     </row>
     <row r="16" spans="1:18" ht="27" customHeight="1">
       <c r="A16" s="22">
         <v>12</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1">
       <c r="A17" s="22">
         <v>13</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1">
       <c r="A18" s="22">
         <v>14</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
     </row>
     <row r="19" spans="1:18" ht="27" customHeight="1">
       <c r="A19" s="22">
         <v>15</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1">
       <c r="A20" s="22">
         <v>16</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="41"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1">
       <c r="A21" s="22">
         <v>17</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
     </row>
     <row r="22" spans="1:18" ht="27" customHeight="1">
       <c r="A22" s="22">
         <v>18</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
     </row>
     <row r="23" spans="1:18" ht="27" customHeight="1"/>
     <row r="24" spans="1:18" ht="27" customHeight="1"/>
@@ -4978,6 +4978,78 @@
     <row r="29" spans="1:18" ht="27" customHeight="1"/>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:O2"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:R4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:R6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:R8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:R9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:R10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:R11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:R12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:R13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:R14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:R15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:R16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:R17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:R18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:R20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:H21"/>
@@ -4986,78 +5058,6 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:R22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:R20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:R17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:R18"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:R15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:R16"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:R13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I14:R14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:R11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:R12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:R9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:R10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:R8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:R5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:R6"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:O2"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:R4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.35433070866141736" footer="0.15748031496062992"/>
@@ -5087,120 +5087,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="57" t="str">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="55" t="str">
         <f>表紙!D6</f>
         <v>Street Biter (STB)</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="45" t="s">
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="43" t="str">
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="59" t="str">
         <f>更新履歴!D5</f>
-        <v>TM</v>
-      </c>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43" t="s">
+        <v>MT</v>
+      </c>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="42" t="str">
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="58" t="str">
         <f>VLOOKUP(MAX(更新履歴!B:B),更新履歴!B:D,3,FALSE)</f>
-        <v>TM</v>
-      </c>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
+        <v>MT</v>
+      </c>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="45" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="54" t="e">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52" t="e">
         <f>RIGHT(表紙!D7,LEN(表紙!D7)-FIND("_",表紙!D7))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="45" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="44">
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="60">
         <f>更新履歴!B5</f>
         <v>45170</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="43" t="s">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="44">
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="60">
         <f>MAX(更新履歴!B:B)</f>
         <v>45170</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I2:X2"/>
-    <mergeCell ref="I1:X1"/>
-    <mergeCell ref="E2:H2"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="AG2:AJ2"/>
     <mergeCell ref="AA1:AD1"/>
@@ -5209,6 +5204,11 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I2:X2"/>
+    <mergeCell ref="I1:X1"/>
+    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.35433070866141736" footer="0.15748031496062992"/>
@@ -5239,120 +5239,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="57" t="str">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="55" t="str">
         <f>表紙!D6</f>
         <v>Street Biter (STB)</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="45" t="s">
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="43" t="str">
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="59" t="str">
         <f>更新履歴!D5</f>
-        <v>TM</v>
-      </c>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43" t="s">
+        <v>MT</v>
+      </c>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="42" t="str">
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="58" t="str">
         <f>VLOOKUP(MAX(更新履歴!B:B),更新履歴!B:D,3,FALSE)</f>
-        <v>TM</v>
-      </c>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
+        <v>MT</v>
+      </c>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="45" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="54" t="e">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52" t="e">
         <f>RIGHT(表紙!D7,LEN(表紙!D7)-FIND("_",表紙!D7))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="45" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="44">
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="60">
         <f>更新履歴!B5</f>
         <v>45170</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="43" t="s">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="44">
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="60">
         <f>MAX(更新履歴!B:B)</f>
         <v>45170</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="60"/>
     </row>
     <row r="44" spans="2:2" ht="15" customHeight="1">
-      <c r="B44" s="60" t="s">
-        <v>34</v>
+      <c r="B44" s="24" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:X2"/>
@@ -5360,11 +5365,6 @@
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
@@ -5396,120 +5396,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="57" t="str">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="55" t="str">
         <f>表紙!D6</f>
         <v>Street Biter (STB)</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="45" t="s">
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="43" t="str">
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="59" t="str">
         <f>更新履歴!D5</f>
-        <v>TM</v>
-      </c>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43" t="s">
+        <v>MT</v>
+      </c>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="42" t="str">
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="58" t="str">
         <f>VLOOKUP(MAX(更新履歴!B:B),更新履歴!B:D,3,FALSE)</f>
-        <v>TM</v>
-      </c>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
+        <v>MT</v>
+      </c>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="45" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="54" t="e">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52" t="e">
         <f>RIGHT(表紙!D7,LEN(表紙!D7)-FIND("_",表紙!D7))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="45" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="44">
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="60">
         <f>更新履歴!B5</f>
         <v>45170</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="43" t="s">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="44">
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="60">
         <f>MAX(更新履歴!B:B)</f>
         <v>45170</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="60"/>
     </row>
     <row r="44" spans="2:2" ht="15" customHeight="1">
-      <c r="B44" s="60" t="s">
-        <v>34</v>
+      <c r="B44" s="24" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:X2"/>
@@ -5517,11 +5522,6 @@
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
@@ -5553,115 +5553,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="57" t="str">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="55" t="str">
         <f>表紙!D6</f>
         <v>Street Biter (STB)</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="45" t="s">
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="43" t="str">
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="59" t="str">
         <f>更新履歴!D5</f>
-        <v>TM</v>
-      </c>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43" t="s">
+        <v>MT</v>
+      </c>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="42" t="str">
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="58" t="str">
         <f>VLOOKUP(MAX(更新履歴!B:B),更新履歴!B:D,3,FALSE)</f>
-        <v>TM</v>
-      </c>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
+        <v>MT</v>
+      </c>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="45" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="54" t="e">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52" t="e">
         <f>RIGHT(表紙!D7,LEN(表紙!D7)-FIND("_",表紙!D7))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="45" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="44">
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="60">
         <f>更新履歴!B5</f>
         <v>45170</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="43" t="s">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="44">
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="60">
         <f>MAX(更新履歴!B:B)</f>
         <v>45170</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:X2"/>
@@ -5669,11 +5674,6 @@
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
@@ -5705,115 +5705,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="57" t="str">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="55" t="str">
         <f>表紙!D6</f>
         <v>Street Biter (STB)</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="45" t="s">
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="43" t="str">
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="59" t="str">
         <f>更新履歴!D5</f>
-        <v>TM</v>
-      </c>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43" t="s">
+        <v>MT</v>
+      </c>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="42" t="str">
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="58" t="str">
         <f>VLOOKUP(MAX(更新履歴!B:B),更新履歴!B:D,3,FALSE)</f>
-        <v>TM</v>
-      </c>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
+        <v>MT</v>
+      </c>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="45" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="54" t="e">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52" t="e">
         <f>RIGHT(表紙!D7,LEN(表紙!D7)-FIND("_",表紙!D7))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="45" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="44">
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="60">
         <f>更新履歴!B5</f>
         <v>45170</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="43" t="s">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="44">
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="60">
         <f>MAX(更新履歴!B:B)</f>
         <v>45170</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:X2"/>
@@ -5821,11 +5826,6 @@
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>

</xml_diff>